<commit_message>
RADP update for Appendix
RADP update for Appendix
</commit_message>
<xml_diff>
--- a/Civilworks cost/IPC Distribution Result/2019-20/IPC Distribution.xlsx
+++ b/Civilworks cost/IPC Distribution Result/2019-20/IPC Distribution.xlsx
@@ -2604,9 +2604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A98" sqref="A98:XFD98"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F107" sqref="F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6424,7 +6424,7 @@
       <c r="G100" s="24"/>
       <c r="H100" s="24"/>
       <c r="I100" s="24"/>
-      <c r="J100" s="24">
+      <c r="J100" s="26">
         <v>3499306</v>
       </c>
       <c r="K100" s="24"/>

</xml_diff>